<commit_message>
updated api testing sheet and corrected numbering
</commit_message>
<xml_diff>
--- a/Templates/TestCases_for_ApiTesting.xlsx
+++ b/Templates/TestCases_for_ApiTesting.xlsx
@@ -4389,7 +4389,7 @@
     </row>
     <row r="4">
       <c r="A4" s="23">
-        <f t="shared" ref="A4:A49" si="1">A3+1</f>
+        <f t="shared" ref="A4:A101" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -5586,7 +5586,10 @@
       <c r="K49" s="22"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="23"/>
+      <c r="A50" s="23">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="B50" s="19" t="s">
         <v>42</v>
       </c>
@@ -5603,7 +5606,10 @@
       <c r="K50" s="22"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="23"/>
+      <c r="A51" s="23">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
       <c r="B51" s="19" t="s">
         <v>42</v>
       </c>
@@ -5624,7 +5630,10 @@
       <c r="K51" s="22"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="23"/>
+      <c r="A52" s="23">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
       <c r="B52" s="19" t="s">
         <v>42</v>
       </c>
@@ -5645,7 +5654,10 @@
       <c r="K52" s="22"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="23"/>
+      <c r="A53" s="23">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
       <c r="B53" s="19" t="s">
         <v>42</v>
       </c>
@@ -5666,7 +5678,10 @@
       <c r="K53" s="22"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="23"/>
+      <c r="A54" s="23">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
       <c r="B54" s="19" t="s">
         <v>42</v>
       </c>
@@ -5687,7 +5702,10 @@
       <c r="K54" s="22"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="23"/>
+      <c r="A55" s="23">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
       <c r="B55" s="19" t="s">
         <v>42</v>
       </c>
@@ -5708,7 +5726,10 @@
       <c r="K55" s="22"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="23"/>
+      <c r="A56" s="23">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
       <c r="B56" s="19" t="s">
         <v>42</v>
       </c>
@@ -5729,7 +5750,10 @@
       <c r="K56" s="22"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="23"/>
+      <c r="A57" s="23">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
       <c r="B57" s="19" t="s">
         <v>42</v>
       </c>
@@ -5750,7 +5774,10 @@
       <c r="K57" s="22"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="23"/>
+      <c r="A58" s="23">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
       <c r="B58" s="19" t="s">
         <v>42</v>
       </c>
@@ -5771,7 +5798,10 @@
       <c r="K58" s="22"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="23"/>
+      <c r="A59" s="23">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
       <c r="B59" s="19" t="s">
         <v>42</v>
       </c>
@@ -5792,7 +5822,10 @@
       <c r="K59" s="22"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="23"/>
+      <c r="A60" s="23">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
       <c r="B60" s="19" t="s">
         <v>42</v>
       </c>
@@ -5813,7 +5846,10 @@
       <c r="K60" s="22"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="23"/>
+      <c r="A61" s="23">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
       <c r="B61" s="19" t="s">
         <v>42</v>
       </c>
@@ -5834,7 +5870,10 @@
       <c r="K61" s="22"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="23"/>
+      <c r="A62" s="23">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
       <c r="B62" s="19" t="s">
         <v>42</v>
       </c>
@@ -5855,7 +5894,10 @@
       <c r="K62" s="22"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="23"/>
+      <c r="A63" s="23">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
       <c r="B63" s="19" t="s">
         <v>42</v>
       </c>
@@ -5877,8 +5919,8 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="23">
-        <f>A49+1</f>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
         <v>42</v>
@@ -5899,8 +5941,8 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="23">
-        <f t="shared" ref="A65:A101" si="2">A64+1</f>
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>42</v>
@@ -5923,8 +5965,8 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="23">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>42</v>
@@ -5947,8 +5989,8 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="23">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="B67" s="19" t="s">
         <v>42</v>
@@ -5971,8 +6013,8 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="23">
-        <f t="shared" si="2"/>
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>42</v>
@@ -5995,8 +6037,8 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="23">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>67</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>42</v>
@@ -6019,8 +6061,8 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="23">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>42</v>
@@ -6043,8 +6085,8 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="23">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B71" s="33" t="s">
         <v>127</v>
@@ -6060,8 +6102,8 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="23">
-        <f t="shared" si="2"/>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="B72" s="34"/>
       <c r="D72" s="22"/>
@@ -6075,8 +6117,8 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="23">
-        <f t="shared" si="2"/>
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="B73" s="34"/>
       <c r="D73" s="22"/>
@@ -6090,8 +6132,8 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="23">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="B74" s="34"/>
       <c r="H74" s="22"/>
@@ -6101,8 +6143,8 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="23">
-        <f t="shared" si="2"/>
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
       <c r="B75" s="34"/>
       <c r="H75" s="22"/>
@@ -6112,8 +6154,8 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="23">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>74</v>
       </c>
       <c r="B76" s="34"/>
       <c r="H76" s="22"/>
@@ -6123,8 +6165,8 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="23">
-        <f t="shared" si="2"/>
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="B77" s="34"/>
       <c r="H77" s="22"/>
@@ -6134,8 +6176,8 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="23">
-        <f t="shared" si="2"/>
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
       <c r="B78" s="34"/>
       <c r="H78" s="22"/>
@@ -6145,8 +6187,8 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="23">
-        <f t="shared" si="2"/>
-        <v>63</v>
+        <f t="shared" si="1"/>
+        <v>77</v>
       </c>
       <c r="B79" s="34"/>
       <c r="H79" s="22"/>
@@ -6156,8 +6198,8 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="23">
-        <f t="shared" si="2"/>
-        <v>64</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
       </c>
       <c r="B80" s="34"/>
       <c r="H80" s="22"/>
@@ -6167,8 +6209,8 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="23">
-        <f t="shared" si="2"/>
-        <v>65</v>
+        <f t="shared" si="1"/>
+        <v>79</v>
       </c>
       <c r="B81" s="34"/>
       <c r="H81" s="22"/>
@@ -6178,8 +6220,8 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="23">
-        <f t="shared" si="2"/>
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="B82" s="34"/>
       <c r="H82" s="22"/>
@@ -6189,8 +6231,8 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="23">
-        <f t="shared" si="2"/>
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>81</v>
       </c>
       <c r="B83" s="34"/>
       <c r="H83" s="22"/>
@@ -6200,8 +6242,8 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="23">
-        <f t="shared" si="2"/>
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>82</v>
       </c>
       <c r="B84" s="34"/>
       <c r="H84" s="22"/>
@@ -6211,8 +6253,8 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="23">
-        <f t="shared" si="2"/>
-        <v>69</v>
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="B85" s="34"/>
       <c r="H85" s="22"/>
@@ -6222,8 +6264,8 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="23">
-        <f t="shared" si="2"/>
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
       <c r="B86" s="34"/>
       <c r="H86" s="22"/>
@@ -6233,8 +6275,8 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="23">
-        <f t="shared" si="2"/>
-        <v>71</v>
+        <f t="shared" si="1"/>
+        <v>85</v>
       </c>
       <c r="B87" s="34"/>
       <c r="H87" s="22"/>
@@ -6244,8 +6286,8 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="23">
-        <f t="shared" si="2"/>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>86</v>
       </c>
       <c r="B88" s="34"/>
       <c r="H88" s="22"/>
@@ -6255,8 +6297,8 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="23">
-        <f t="shared" si="2"/>
-        <v>73</v>
+        <f t="shared" si="1"/>
+        <v>87</v>
       </c>
       <c r="B89" s="34"/>
       <c r="H89" s="22"/>
@@ -6266,8 +6308,8 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="23">
-        <f t="shared" si="2"/>
-        <v>74</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="B90" s="34"/>
       <c r="H90" s="22"/>
@@ -6277,8 +6319,8 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="23">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>89</v>
       </c>
       <c r="B91" s="34"/>
       <c r="H91" s="22"/>
@@ -6288,8 +6330,8 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="23">
-        <f t="shared" si="2"/>
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="B92" s="34"/>
       <c r="H92" s="22"/>
@@ -6299,8 +6341,8 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="23">
-        <f t="shared" si="2"/>
-        <v>77</v>
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
       <c r="B93" s="34"/>
       <c r="H93" s="22"/>
@@ -6310,8 +6352,8 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="23">
-        <f t="shared" si="2"/>
-        <v>78</v>
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="B94" s="34"/>
       <c r="C94" s="34"/>
@@ -6322,8 +6364,8 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="23">
-        <f t="shared" si="2"/>
-        <v>79</v>
+        <f t="shared" si="1"/>
+        <v>93</v>
       </c>
       <c r="B95" s="34"/>
       <c r="H95" s="22"/>
@@ -6333,8 +6375,8 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="23">
-        <f t="shared" si="2"/>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>94</v>
       </c>
       <c r="B96" s="34"/>
       <c r="H96" s="22"/>
@@ -6344,8 +6386,8 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="23">
-        <f t="shared" si="2"/>
-        <v>81</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="B97" s="34"/>
       <c r="H97" s="22"/>
@@ -6355,8 +6397,8 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="23">
-        <f t="shared" si="2"/>
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
       <c r="B98" s="34"/>
       <c r="H98" s="22"/>
@@ -6366,8 +6408,8 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="23">
-        <f t="shared" si="2"/>
-        <v>83</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="B99" s="34"/>
       <c r="H99" s="22"/>
@@ -6377,8 +6419,8 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="23">
-        <f t="shared" si="2"/>
-        <v>84</v>
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="B100" s="34"/>
       <c r="H100" s="22"/>
@@ -6388,8 +6430,8 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="23">
-        <f t="shared" si="2"/>
-        <v>85</v>
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
       <c r="B101" s="34"/>
       <c r="H101" s="22"/>
@@ -6408,7 +6450,7 @@
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="23">
         <f>A101+1</f>
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B103" s="34"/>
       <c r="H103" s="22"/>
@@ -6418,8 +6460,8 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="23">
-        <f t="shared" ref="A104:A121" si="3">A103+1</f>
-        <v>87</v>
+        <f t="shared" ref="A104:A121" si="2">A103+1</f>
+        <v>101</v>
       </c>
       <c r="B104" s="34"/>
       <c r="H104" s="22"/>
@@ -6429,8 +6471,8 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="23">
-        <f t="shared" si="3"/>
-        <v>88</v>
+        <f t="shared" si="2"/>
+        <v>102</v>
       </c>
       <c r="B105" s="34"/>
       <c r="H105" s="22"/>
@@ -6440,8 +6482,8 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="23">
-        <f t="shared" si="3"/>
-        <v>89</v>
+        <f t="shared" si="2"/>
+        <v>103</v>
       </c>
       <c r="B106" s="34"/>
       <c r="H106" s="22"/>
@@ -6451,8 +6493,8 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="23">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>104</v>
       </c>
       <c r="B107" s="34"/>
       <c r="H107" s="22"/>
@@ -6462,8 +6504,8 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="23">
-        <f t="shared" si="3"/>
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>105</v>
       </c>
       <c r="B108" s="34"/>
       <c r="H108" s="22"/>
@@ -6473,8 +6515,8 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="23">
-        <f t="shared" si="3"/>
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>106</v>
       </c>
       <c r="B109" s="34"/>
       <c r="C109" s="34"/>
@@ -6485,8 +6527,8 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="23">
-        <f t="shared" si="3"/>
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>107</v>
       </c>
       <c r="B110" s="34"/>
       <c r="H110" s="22"/>
@@ -6496,8 +6538,8 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="23">
-        <f t="shared" si="3"/>
-        <v>94</v>
+        <f t="shared" si="2"/>
+        <v>108</v>
       </c>
       <c r="B111" s="34"/>
       <c r="H111" s="22"/>
@@ -6507,8 +6549,8 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="23">
-        <f t="shared" si="3"/>
-        <v>95</v>
+        <f t="shared" si="2"/>
+        <v>109</v>
       </c>
       <c r="B112" s="34"/>
       <c r="H112" s="22"/>
@@ -6518,8 +6560,8 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="23">
-        <f t="shared" si="3"/>
-        <v>96</v>
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="B113" s="34"/>
       <c r="H113" s="22"/>
@@ -6529,8 +6571,8 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="23">
-        <f t="shared" si="3"/>
-        <v>97</v>
+        <f t="shared" si="2"/>
+        <v>111</v>
       </c>
       <c r="B114" s="34"/>
       <c r="H114" s="22"/>
@@ -6540,8 +6582,8 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="23">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <f t="shared" si="2"/>
+        <v>112</v>
       </c>
       <c r="B115" s="34"/>
       <c r="H115" s="22"/>
@@ -6551,8 +6593,8 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="23">
-        <f t="shared" si="3"/>
-        <v>99</v>
+        <f t="shared" si="2"/>
+        <v>113</v>
       </c>
       <c r="B116" s="34"/>
       <c r="H116" s="22"/>
@@ -6562,8 +6604,8 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="23">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>114</v>
       </c>
       <c r="B117" s="34"/>
       <c r="H117" s="22"/>
@@ -6573,8 +6615,8 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="23">
-        <f t="shared" si="3"/>
-        <v>101</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="B118" s="34"/>
       <c r="H118" s="22"/>
@@ -6584,8 +6626,8 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="23">
-        <f t="shared" si="3"/>
-        <v>102</v>
+        <f t="shared" si="2"/>
+        <v>116</v>
       </c>
       <c r="B119" s="34"/>
       <c r="H119" s="22"/>
@@ -6595,8 +6637,8 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="23">
-        <f t="shared" si="3"/>
-        <v>103</v>
+        <f t="shared" si="2"/>
+        <v>117</v>
       </c>
       <c r="B120" s="34"/>
       <c r="H120" s="22"/>
@@ -6606,8 +6648,8 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="23">
-        <f t="shared" si="3"/>
-        <v>104</v>
+        <f t="shared" si="2"/>
+        <v>118</v>
       </c>
       <c r="B121" s="34" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Updated readme with more blog links and corrected numbering in API tests sheet (#28)
* updated api testing sheet and corrected numbering

* updated readme with blog links
</commit_message>
<xml_diff>
--- a/Templates/TestCases_for_ApiTesting.xlsx
+++ b/Templates/TestCases_for_ApiTesting.xlsx
@@ -4389,7 +4389,7 @@
     </row>
     <row r="4">
       <c r="A4" s="23">
-        <f t="shared" ref="A4:A49" si="1">A3+1</f>
+        <f t="shared" ref="A4:A101" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -5586,7 +5586,10 @@
       <c r="K49" s="22"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="23"/>
+      <c r="A50" s="23">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="B50" s="19" t="s">
         <v>42</v>
       </c>
@@ -5603,7 +5606,10 @@
       <c r="K50" s="22"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="23"/>
+      <c r="A51" s="23">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
       <c r="B51" s="19" t="s">
         <v>42</v>
       </c>
@@ -5624,7 +5630,10 @@
       <c r="K51" s="22"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="23"/>
+      <c r="A52" s="23">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
       <c r="B52" s="19" t="s">
         <v>42</v>
       </c>
@@ -5645,7 +5654,10 @@
       <c r="K52" s="22"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="23"/>
+      <c r="A53" s="23">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
       <c r="B53" s="19" t="s">
         <v>42</v>
       </c>
@@ -5666,7 +5678,10 @@
       <c r="K53" s="22"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="23"/>
+      <c r="A54" s="23">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
       <c r="B54" s="19" t="s">
         <v>42</v>
       </c>
@@ -5687,7 +5702,10 @@
       <c r="K54" s="22"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="23"/>
+      <c r="A55" s="23">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
       <c r="B55" s="19" t="s">
         <v>42</v>
       </c>
@@ -5708,7 +5726,10 @@
       <c r="K55" s="22"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="23"/>
+      <c r="A56" s="23">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
       <c r="B56" s="19" t="s">
         <v>42</v>
       </c>
@@ -5729,7 +5750,10 @@
       <c r="K56" s="22"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="23"/>
+      <c r="A57" s="23">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
       <c r="B57" s="19" t="s">
         <v>42</v>
       </c>
@@ -5750,7 +5774,10 @@
       <c r="K57" s="22"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="23"/>
+      <c r="A58" s="23">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
       <c r="B58" s="19" t="s">
         <v>42</v>
       </c>
@@ -5771,7 +5798,10 @@
       <c r="K58" s="22"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="23"/>
+      <c r="A59" s="23">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
       <c r="B59" s="19" t="s">
         <v>42</v>
       </c>
@@ -5792,7 +5822,10 @@
       <c r="K59" s="22"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="23"/>
+      <c r="A60" s="23">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
       <c r="B60" s="19" t="s">
         <v>42</v>
       </c>
@@ -5813,7 +5846,10 @@
       <c r="K60" s="22"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="23"/>
+      <c r="A61" s="23">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
       <c r="B61" s="19" t="s">
         <v>42</v>
       </c>
@@ -5834,7 +5870,10 @@
       <c r="K61" s="22"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="23"/>
+      <c r="A62" s="23">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
       <c r="B62" s="19" t="s">
         <v>42</v>
       </c>
@@ -5855,7 +5894,10 @@
       <c r="K62" s="22"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="23"/>
+      <c r="A63" s="23">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
       <c r="B63" s="19" t="s">
         <v>42</v>
       </c>
@@ -5877,8 +5919,8 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="23">
-        <f>A49+1</f>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
         <v>42</v>
@@ -5899,8 +5941,8 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="23">
-        <f t="shared" ref="A65:A101" si="2">A64+1</f>
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>42</v>
@@ -5923,8 +5965,8 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="23">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>42</v>
@@ -5947,8 +5989,8 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="23">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="B67" s="19" t="s">
         <v>42</v>
@@ -5971,8 +6013,8 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="23">
-        <f t="shared" si="2"/>
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>42</v>
@@ -5995,8 +6037,8 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="23">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>67</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>42</v>
@@ -6019,8 +6061,8 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="23">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>42</v>
@@ -6043,8 +6085,8 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="23">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B71" s="33" t="s">
         <v>127</v>
@@ -6060,8 +6102,8 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="23">
-        <f t="shared" si="2"/>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="B72" s="34"/>
       <c r="D72" s="22"/>
@@ -6075,8 +6117,8 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="23">
-        <f t="shared" si="2"/>
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="B73" s="34"/>
       <c r="D73" s="22"/>
@@ -6090,8 +6132,8 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="23">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="B74" s="34"/>
       <c r="H74" s="22"/>
@@ -6101,8 +6143,8 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="23">
-        <f t="shared" si="2"/>
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
       <c r="B75" s="34"/>
       <c r="H75" s="22"/>
@@ -6112,8 +6154,8 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="23">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>74</v>
       </c>
       <c r="B76" s="34"/>
       <c r="H76" s="22"/>
@@ -6123,8 +6165,8 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="23">
-        <f t="shared" si="2"/>
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="B77" s="34"/>
       <c r="H77" s="22"/>
@@ -6134,8 +6176,8 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="23">
-        <f t="shared" si="2"/>
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
       <c r="B78" s="34"/>
       <c r="H78" s="22"/>
@@ -6145,8 +6187,8 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="23">
-        <f t="shared" si="2"/>
-        <v>63</v>
+        <f t="shared" si="1"/>
+        <v>77</v>
       </c>
       <c r="B79" s="34"/>
       <c r="H79" s="22"/>
@@ -6156,8 +6198,8 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="23">
-        <f t="shared" si="2"/>
-        <v>64</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
       </c>
       <c r="B80" s="34"/>
       <c r="H80" s="22"/>
@@ -6167,8 +6209,8 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="23">
-        <f t="shared" si="2"/>
-        <v>65</v>
+        <f t="shared" si="1"/>
+        <v>79</v>
       </c>
       <c r="B81" s="34"/>
       <c r="H81" s="22"/>
@@ -6178,8 +6220,8 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="23">
-        <f t="shared" si="2"/>
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="B82" s="34"/>
       <c r="H82" s="22"/>
@@ -6189,8 +6231,8 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="23">
-        <f t="shared" si="2"/>
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>81</v>
       </c>
       <c r="B83" s="34"/>
       <c r="H83" s="22"/>
@@ -6200,8 +6242,8 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="23">
-        <f t="shared" si="2"/>
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>82</v>
       </c>
       <c r="B84" s="34"/>
       <c r="H84" s="22"/>
@@ -6211,8 +6253,8 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="23">
-        <f t="shared" si="2"/>
-        <v>69</v>
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="B85" s="34"/>
       <c r="H85" s="22"/>
@@ -6222,8 +6264,8 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="23">
-        <f t="shared" si="2"/>
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
       <c r="B86" s="34"/>
       <c r="H86" s="22"/>
@@ -6233,8 +6275,8 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="23">
-        <f t="shared" si="2"/>
-        <v>71</v>
+        <f t="shared" si="1"/>
+        <v>85</v>
       </c>
       <c r="B87" s="34"/>
       <c r="H87" s="22"/>
@@ -6244,8 +6286,8 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="23">
-        <f t="shared" si="2"/>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>86</v>
       </c>
       <c r="B88" s="34"/>
       <c r="H88" s="22"/>
@@ -6255,8 +6297,8 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="23">
-        <f t="shared" si="2"/>
-        <v>73</v>
+        <f t="shared" si="1"/>
+        <v>87</v>
       </c>
       <c r="B89" s="34"/>
       <c r="H89" s="22"/>
@@ -6266,8 +6308,8 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="23">
-        <f t="shared" si="2"/>
-        <v>74</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="B90" s="34"/>
       <c r="H90" s="22"/>
@@ -6277,8 +6319,8 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="23">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>89</v>
       </c>
       <c r="B91" s="34"/>
       <c r="H91" s="22"/>
@@ -6288,8 +6330,8 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="23">
-        <f t="shared" si="2"/>
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="B92" s="34"/>
       <c r="H92" s="22"/>
@@ -6299,8 +6341,8 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="23">
-        <f t="shared" si="2"/>
-        <v>77</v>
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
       <c r="B93" s="34"/>
       <c r="H93" s="22"/>
@@ -6310,8 +6352,8 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="23">
-        <f t="shared" si="2"/>
-        <v>78</v>
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="B94" s="34"/>
       <c r="C94" s="34"/>
@@ -6322,8 +6364,8 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="23">
-        <f t="shared" si="2"/>
-        <v>79</v>
+        <f t="shared" si="1"/>
+        <v>93</v>
       </c>
       <c r="B95" s="34"/>
       <c r="H95" s="22"/>
@@ -6333,8 +6375,8 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="23">
-        <f t="shared" si="2"/>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>94</v>
       </c>
       <c r="B96" s="34"/>
       <c r="H96" s="22"/>
@@ -6344,8 +6386,8 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="23">
-        <f t="shared" si="2"/>
-        <v>81</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="B97" s="34"/>
       <c r="H97" s="22"/>
@@ -6355,8 +6397,8 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="23">
-        <f t="shared" si="2"/>
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
       <c r="B98" s="34"/>
       <c r="H98" s="22"/>
@@ -6366,8 +6408,8 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="23">
-        <f t="shared" si="2"/>
-        <v>83</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="B99" s="34"/>
       <c r="H99" s="22"/>
@@ -6377,8 +6419,8 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="23">
-        <f t="shared" si="2"/>
-        <v>84</v>
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="B100" s="34"/>
       <c r="H100" s="22"/>
@@ -6388,8 +6430,8 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="23">
-        <f t="shared" si="2"/>
-        <v>85</v>
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
       <c r="B101" s="34"/>
       <c r="H101" s="22"/>
@@ -6408,7 +6450,7 @@
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="23">
         <f>A101+1</f>
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B103" s="34"/>
       <c r="H103" s="22"/>
@@ -6418,8 +6460,8 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="23">
-        <f t="shared" ref="A104:A121" si="3">A103+1</f>
-        <v>87</v>
+        <f t="shared" ref="A104:A121" si="2">A103+1</f>
+        <v>101</v>
       </c>
       <c r="B104" s="34"/>
       <c r="H104" s="22"/>
@@ -6429,8 +6471,8 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="23">
-        <f t="shared" si="3"/>
-        <v>88</v>
+        <f t="shared" si="2"/>
+        <v>102</v>
       </c>
       <c r="B105" s="34"/>
       <c r="H105" s="22"/>
@@ -6440,8 +6482,8 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="23">
-        <f t="shared" si="3"/>
-        <v>89</v>
+        <f t="shared" si="2"/>
+        <v>103</v>
       </c>
       <c r="B106" s="34"/>
       <c r="H106" s="22"/>
@@ -6451,8 +6493,8 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="23">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>104</v>
       </c>
       <c r="B107" s="34"/>
       <c r="H107" s="22"/>
@@ -6462,8 +6504,8 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="23">
-        <f t="shared" si="3"/>
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>105</v>
       </c>
       <c r="B108" s="34"/>
       <c r="H108" s="22"/>
@@ -6473,8 +6515,8 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="23">
-        <f t="shared" si="3"/>
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>106</v>
       </c>
       <c r="B109" s="34"/>
       <c r="C109" s="34"/>
@@ -6485,8 +6527,8 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="23">
-        <f t="shared" si="3"/>
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>107</v>
       </c>
       <c r="B110" s="34"/>
       <c r="H110" s="22"/>
@@ -6496,8 +6538,8 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="23">
-        <f t="shared" si="3"/>
-        <v>94</v>
+        <f t="shared" si="2"/>
+        <v>108</v>
       </c>
       <c r="B111" s="34"/>
       <c r="H111" s="22"/>
@@ -6507,8 +6549,8 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="23">
-        <f t="shared" si="3"/>
-        <v>95</v>
+        <f t="shared" si="2"/>
+        <v>109</v>
       </c>
       <c r="B112" s="34"/>
       <c r="H112" s="22"/>
@@ -6518,8 +6560,8 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="23">
-        <f t="shared" si="3"/>
-        <v>96</v>
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="B113" s="34"/>
       <c r="H113" s="22"/>
@@ -6529,8 +6571,8 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="23">
-        <f t="shared" si="3"/>
-        <v>97</v>
+        <f t="shared" si="2"/>
+        <v>111</v>
       </c>
       <c r="B114" s="34"/>
       <c r="H114" s="22"/>
@@ -6540,8 +6582,8 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="23">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <f t="shared" si="2"/>
+        <v>112</v>
       </c>
       <c r="B115" s="34"/>
       <c r="H115" s="22"/>
@@ -6551,8 +6593,8 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="23">
-        <f t="shared" si="3"/>
-        <v>99</v>
+        <f t="shared" si="2"/>
+        <v>113</v>
       </c>
       <c r="B116" s="34"/>
       <c r="H116" s="22"/>
@@ -6562,8 +6604,8 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="23">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>114</v>
       </c>
       <c r="B117" s="34"/>
       <c r="H117" s="22"/>
@@ -6573,8 +6615,8 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="23">
-        <f t="shared" si="3"/>
-        <v>101</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="B118" s="34"/>
       <c r="H118" s="22"/>
@@ -6584,8 +6626,8 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="23">
-        <f t="shared" si="3"/>
-        <v>102</v>
+        <f t="shared" si="2"/>
+        <v>116</v>
       </c>
       <c r="B119" s="34"/>
       <c r="H119" s="22"/>
@@ -6595,8 +6637,8 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="23">
-        <f t="shared" si="3"/>
-        <v>103</v>
+        <f t="shared" si="2"/>
+        <v>117</v>
       </c>
       <c r="B120" s="34"/>
       <c r="H120" s="22"/>
@@ -6606,8 +6648,8 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="23">
-        <f t="shared" si="3"/>
-        <v>104</v>
+        <f t="shared" si="2"/>
+        <v>118</v>
       </c>
       <c r="B121" s="34" t="s">
         <v>127</v>

</xml_diff>